<commit_message>
Atualizado por script em 03-01-2024 02:45
</commit_message>
<xml_diff>
--- a/2023/spain_laliga_2023-2024.xlsx
+++ b/2023/spain_laliga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V183"/>
+  <dimension ref="A1:V184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6185,15 +6185,15 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Ath Bilbao</t>
+          <t>Villarreal</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Getafe</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -6208,48 +6208,48 @@
         </is>
       </c>
       <c r="L63" t="n">
-        <v>1.53</v>
+        <v>2.17</v>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>27/09/2023 18:31</t>
+          <t>27/09/2023 18:51</t>
         </is>
       </c>
       <c r="N63" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>17/09/2023 09:02</t>
+        </is>
+      </c>
+      <c r="P63" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>27/09/2023 18:51</t>
+        </is>
+      </c>
+      <c r="R63" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>17/09/2023 09:02</t>
+        </is>
+      </c>
+      <c r="T63" t="n">
         <v>3.42</v>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>17/09/2023 09:02</t>
-        </is>
-      </c>
-      <c r="P63" t="n">
-        <v>4.06</v>
-      </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>27/09/2023 18:49</t>
-        </is>
-      </c>
-      <c r="R63" t="n">
-        <v>5.44</v>
-      </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>17/09/2023 09:02</t>
-        </is>
-      </c>
-      <c r="T63" t="n">
-        <v>7.73</v>
-      </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>27/09/2023 18:49</t>
+          <t>27/09/2023 18:51</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/ath-bilbao-getafe/zgsFCYIT/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/villarreal-girona/80EuTg3A/</t>
         </is>
       </c>
     </row>
@@ -6369,15 +6369,15 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Villarreal</t>
+          <t>Ath Bilbao</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Girona</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -6392,15 +6392,15 @@
         </is>
       </c>
       <c r="L65" t="n">
-        <v>2.17</v>
+        <v>1.53</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>27/09/2023 18:51</t>
+          <t>27/09/2023 18:31</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>4.14</v>
+        <v>3.42</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -6408,15 +6408,15 @@
         </is>
       </c>
       <c r="P65" t="n">
-        <v>3.72</v>
+        <v>4.06</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>27/09/2023 18:51</t>
+          <t>27/09/2023 18:49</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>4.72</v>
+        <v>5.44</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
@@ -6424,16 +6424,16 @@
         </is>
       </c>
       <c r="T65" t="n">
-        <v>3.42</v>
+        <v>7.73</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>27/09/2023 18:51</t>
+          <t>27/09/2023 18:49</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/villarreal-girona/80EuTg3A/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/ath-bilbao-getafe/zgsFCYIT/</t>
         </is>
       </c>
     </row>
@@ -6461,7 +6461,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Cadiz CF</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="G66" t="n">
@@ -6469,14 +6469,14 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Rayo Vallecano</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="I66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J66" t="n">
-        <v>2.59</v>
+        <v>2.33</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
@@ -6484,15 +6484,15 @@
         </is>
       </c>
       <c r="L66" t="n">
-        <v>2.72</v>
+        <v>2.57</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>27/09/2023 21:19</t>
+          <t>27/09/2023 21:27</t>
         </is>
       </c>
       <c r="N66" t="n">
-        <v>3.06</v>
+        <v>3.14</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -6500,15 +6500,15 @@
         </is>
       </c>
       <c r="P66" t="n">
-        <v>3.11</v>
+        <v>3.02</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>27/09/2023 21:17</t>
+          <t>27/09/2023 21:27</t>
         </is>
       </c>
       <c r="R66" t="n">
-        <v>3.11</v>
+        <v>3.26</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
@@ -6516,16 +6516,16 @@
         </is>
       </c>
       <c r="T66" t="n">
-        <v>3</v>
+        <v>3.31</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>27/09/2023 21:30</t>
+          <t>27/09/2023 21:27</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/cadiz-rayo-vallecano/CEYt8hRp/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/valencia-real-sociedad/M3IqSDIG/</t>
         </is>
       </c>
     </row>
@@ -6553,7 +6553,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>Cadiz CF</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -6561,14 +6561,14 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Real Sociedad</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="I67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J67" t="n">
-        <v>2.33</v>
+        <v>2.59</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
@@ -6576,15 +6576,15 @@
         </is>
       </c>
       <c r="L67" t="n">
-        <v>2.57</v>
+        <v>2.72</v>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>27/09/2023 21:27</t>
+          <t>27/09/2023 21:19</t>
         </is>
       </c>
       <c r="N67" t="n">
-        <v>3.14</v>
+        <v>3.06</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -6592,15 +6592,15 @@
         </is>
       </c>
       <c r="P67" t="n">
-        <v>3.02</v>
+        <v>3.11</v>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>27/09/2023 21:27</t>
+          <t>27/09/2023 21:17</t>
         </is>
       </c>
       <c r="R67" t="n">
-        <v>3.26</v>
+        <v>3.11</v>
       </c>
       <c r="S67" t="inlineStr">
         <is>
@@ -6608,16 +6608,16 @@
         </is>
       </c>
       <c r="T67" t="n">
-        <v>3.31</v>
+        <v>3</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>27/09/2023 21:27</t>
+          <t>27/09/2023 21:30</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/valencia-real-sociedad/M3IqSDIG/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/cadiz-rayo-vallecano/CEYt8hRp/</t>
         </is>
       </c>
     </row>
@@ -17290,6 +17290,98 @@
       <c r="V183" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/spain/laliga/real-sociedad-alaves/GrNqhGfT/</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>spain</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>laliga</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E184" s="2" t="n">
+        <v>45293.89583333334</v>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="G184" t="n">
+        <v>3</v>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="I184" t="n">
+        <v>1</v>
+      </c>
+      <c r="J184" t="n">
+        <v>2</v>
+      </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="L184" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t>02/01/2024 21:29</t>
+        </is>
+      </c>
+      <c r="N184" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="O184" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="P184" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="Q184" t="inlineStr">
+        <is>
+          <t>02/01/2024 21:14</t>
+        </is>
+      </c>
+      <c r="R184" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="S184" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="T184" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="U184" t="inlineStr">
+        <is>
+          <t>02/01/2024 21:29</t>
+        </is>
+      </c>
+      <c r="V184" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/spain/laliga/valencia-villarreal/bskYZGYp/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 04-01-2024 02:45
</commit_message>
<xml_diff>
--- a/2023/spain_laliga_2023-2024.xlsx
+++ b/2023/spain_laliga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V187"/>
+  <dimension ref="A1:V188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16213,22 +16213,22 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>Granada CF</t>
+          <t>Atl. Madrid</t>
         </is>
       </c>
       <c r="G172" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>Sevilla</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="I172" t="n">
         <v>3</v>
       </c>
       <c r="J172" t="n">
-        <v>2.76</v>
+        <v>1.31</v>
       </c>
       <c r="K172" t="inlineStr">
         <is>
@@ -16236,15 +16236,15 @@
         </is>
       </c>
       <c r="L172" t="n">
-        <v>3.12</v>
+        <v>1.48</v>
       </c>
       <c r="M172" t="inlineStr">
         <is>
-          <t>19/12/2023 21:27</t>
+          <t>19/12/2023 21:28</t>
         </is>
       </c>
       <c r="N172" t="n">
-        <v>3.33</v>
+        <v>4.91</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -16252,15 +16252,15 @@
         </is>
       </c>
       <c r="P172" t="n">
-        <v>3.17</v>
+        <v>4.54</v>
       </c>
       <c r="Q172" t="inlineStr">
         <is>
-          <t>19/12/2023 21:05</t>
+          <t>19/12/2023 21:29</t>
         </is>
       </c>
       <c r="R172" t="n">
-        <v>2.48</v>
+        <v>9</v>
       </c>
       <c r="S172" t="inlineStr">
         <is>
@@ -16268,16 +16268,16 @@
         </is>
       </c>
       <c r="T172" t="n">
-        <v>2.55</v>
+        <v>7.35</v>
       </c>
       <c r="U172" t="inlineStr">
         <is>
-          <t>19/12/2023 21:25</t>
+          <t>19/12/2023 21:29</t>
         </is>
       </c>
       <c r="V172" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/granada-cf-sevilla/KhVmeR4g/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/atl-madrid-getafe/EwmSwQZI/</t>
         </is>
       </c>
     </row>
@@ -16305,22 +16305,22 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>Atl. Madrid</t>
+          <t>Granada CF</t>
         </is>
       </c>
       <c r="G173" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>Getafe</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="I173" t="n">
         <v>3</v>
       </c>
       <c r="J173" t="n">
-        <v>1.31</v>
+        <v>2.76</v>
       </c>
       <c r="K173" t="inlineStr">
         <is>
@@ -16328,15 +16328,15 @@
         </is>
       </c>
       <c r="L173" t="n">
-        <v>1.48</v>
+        <v>3.12</v>
       </c>
       <c r="M173" t="inlineStr">
         <is>
-          <t>19/12/2023 21:28</t>
+          <t>19/12/2023 21:27</t>
         </is>
       </c>
       <c r="N173" t="n">
-        <v>4.91</v>
+        <v>3.33</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -16344,15 +16344,15 @@
         </is>
       </c>
       <c r="P173" t="n">
-        <v>4.54</v>
+        <v>3.17</v>
       </c>
       <c r="Q173" t="inlineStr">
         <is>
-          <t>19/12/2023 21:29</t>
+          <t>19/12/2023 21:05</t>
         </is>
       </c>
       <c r="R173" t="n">
-        <v>9</v>
+        <v>2.48</v>
       </c>
       <c r="S173" t="inlineStr">
         <is>
@@ -16360,16 +16360,16 @@
         </is>
       </c>
       <c r="T173" t="n">
-        <v>7.35</v>
+        <v>2.55</v>
       </c>
       <c r="U173" t="inlineStr">
         <is>
-          <t>19/12/2023 21:29</t>
+          <t>19/12/2023 21:25</t>
         </is>
       </c>
       <c r="V173" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/atl-madrid-getafe/EwmSwQZI/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/granada-cf-sevilla/KhVmeR4g/</t>
         </is>
       </c>
     </row>
@@ -17501,22 +17501,22 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>Celta Vigo</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="G186" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Betis</t>
+          <t>Mallorca</t>
         </is>
       </c>
       <c r="I186" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J186" t="n">
-        <v>1.95</v>
+        <v>1.17</v>
       </c>
       <c r="K186" t="inlineStr">
         <is>
@@ -17524,48 +17524,48 @@
         </is>
       </c>
       <c r="L186" t="n">
-        <v>2.21</v>
+        <v>1.22</v>
       </c>
       <c r="M186" t="inlineStr">
         <is>
+          <t>03/01/2024 19:10</t>
+        </is>
+      </c>
+      <c r="N186" t="n">
+        <v>6.63</v>
+      </c>
+      <c r="O186" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="P186" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="Q186" t="inlineStr">
+        <is>
           <t>03/01/2024 19:14</t>
         </is>
       </c>
-      <c r="N186" t="n">
-        <v>3.47</v>
-      </c>
-      <c r="O186" t="inlineStr">
+      <c r="R186" t="n">
+        <v>12.67</v>
+      </c>
+      <c r="S186" t="inlineStr">
         <is>
           <t>17/12/2024 18:03</t>
         </is>
       </c>
-      <c r="P186" t="n">
-        <v>3.31</v>
-      </c>
-      <c r="Q186" t="inlineStr">
+      <c r="T186" t="n">
+        <v>13.93</v>
+      </c>
+      <c r="U186" t="inlineStr">
         <is>
           <t>03/01/2024 19:14</t>
         </is>
       </c>
-      <c r="R186" t="n">
-        <v>3.77</v>
-      </c>
-      <c r="S186" t="inlineStr">
-        <is>
-          <t>17/12/2024 18:03</t>
-        </is>
-      </c>
-      <c r="T186" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="U186" t="inlineStr">
-        <is>
-          <t>03/01/2024 19:14</t>
-        </is>
-      </c>
       <c r="V186" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/celta-vigo-betis/URKXfIAA/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/real-madrid-mallorca/xhOugduN/</t>
         </is>
       </c>
     </row>
@@ -17593,22 +17593,22 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Celta Vigo</t>
         </is>
       </c>
       <c r="G187" t="n">
+        <v>2</v>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>Betis</t>
+        </is>
+      </c>
+      <c r="I187" t="n">
         <v>1</v>
       </c>
-      <c r="H187" t="inlineStr">
-        <is>
-          <t>Mallorca</t>
-        </is>
-      </c>
-      <c r="I187" t="n">
-        <v>0</v>
-      </c>
       <c r="J187" t="n">
-        <v>1.17</v>
+        <v>1.95</v>
       </c>
       <c r="K187" t="inlineStr">
         <is>
@@ -17616,15 +17616,15 @@
         </is>
       </c>
       <c r="L187" t="n">
-        <v>1.22</v>
+        <v>2.21</v>
       </c>
       <c r="M187" t="inlineStr">
         <is>
-          <t>03/01/2024 19:10</t>
+          <t>03/01/2024 19:14</t>
         </is>
       </c>
       <c r="N187" t="n">
-        <v>6.63</v>
+        <v>3.47</v>
       </c>
       <c r="O187" t="inlineStr">
         <is>
@@ -17632,7 +17632,7 @@
         </is>
       </c>
       <c r="P187" t="n">
-        <v>6.75</v>
+        <v>3.31</v>
       </c>
       <c r="Q187" t="inlineStr">
         <is>
@@ -17640,7 +17640,7 @@
         </is>
       </c>
       <c r="R187" t="n">
-        <v>12.67</v>
+        <v>3.77</v>
       </c>
       <c r="S187" t="inlineStr">
         <is>
@@ -17648,7 +17648,7 @@
         </is>
       </c>
       <c r="T187" t="n">
-        <v>13.93</v>
+        <v>3.67</v>
       </c>
       <c r="U187" t="inlineStr">
         <is>
@@ -17657,7 +17657,99 @@
       </c>
       <c r="V187" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/real-madrid-mallorca/xhOugduN/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/celta-vigo-betis/URKXfIAA/</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>spain</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>laliga</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E188" s="2" t="n">
+        <v>45294.89583333334</v>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Girona</t>
+        </is>
+      </c>
+      <c r="G188" t="n">
+        <v>4</v>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>Atl. Madrid</t>
+        </is>
+      </c>
+      <c r="I188" t="n">
+        <v>3</v>
+      </c>
+      <c r="J188" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="L188" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="M188" t="inlineStr">
+        <is>
+          <t>03/01/2024 21:02</t>
+        </is>
+      </c>
+      <c r="N188" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="O188" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="P188" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="Q188" t="inlineStr">
+        <is>
+          <t>03/01/2024 21:28</t>
+        </is>
+      </c>
+      <c r="R188" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="S188" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="T188" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="U188" t="inlineStr">
+        <is>
+          <t>03/01/2024 21:28</t>
+        </is>
+      </c>
+      <c r="V188" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/spain/laliga/girona-atl-madrid/8CWOdvtb/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 05-01-2024 02:45
</commit_message>
<xml_diff>
--- a/2023/spain_laliga_2023-2024.xlsx
+++ b/2023/spain_laliga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V190"/>
+  <dimension ref="A1:V191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16673,22 +16673,22 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Betis</t>
+          <t>Cadiz CF</t>
         </is>
       </c>
       <c r="G177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Girona</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="I177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J177" t="n">
-        <v>2.31</v>
+        <v>4.08</v>
       </c>
       <c r="K177" t="inlineStr">
         <is>
@@ -16696,39 +16696,39 @@
         </is>
       </c>
       <c r="L177" t="n">
-        <v>2.67</v>
+        <v>6.27</v>
       </c>
       <c r="M177" t="inlineStr">
         <is>
+          <t>21/12/2023 18:57</t>
+        </is>
+      </c>
+      <c r="N177" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="O177" t="inlineStr">
+        <is>
+          <t>10/12/2023 10:02</t>
+        </is>
+      </c>
+      <c r="P177" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="Q177" t="inlineStr">
+        <is>
           <t>21/12/2023 18:59</t>
         </is>
       </c>
-      <c r="N177" t="n">
-        <v>3.42</v>
-      </c>
-      <c r="O177" t="inlineStr">
+      <c r="R177" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="S177" t="inlineStr">
         <is>
           <t>10/12/2023 10:02</t>
         </is>
       </c>
-      <c r="P177" t="n">
-        <v>3.55</v>
-      </c>
-      <c r="Q177" t="inlineStr">
-        <is>
-          <t>21/12/2023 18:59</t>
-        </is>
-      </c>
-      <c r="R177" t="n">
-        <v>2.96</v>
-      </c>
-      <c r="S177" t="inlineStr">
-        <is>
-          <t>10/12/2023 10:02</t>
-        </is>
-      </c>
       <c r="T177" t="n">
-        <v>2.69</v>
+        <v>1.69</v>
       </c>
       <c r="U177" t="inlineStr">
         <is>
@@ -16737,7 +16737,7 @@
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/betis-girona/Sfj929CJ/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/cadiz-real-sociedad/6okD1TRP/</t>
         </is>
       </c>
     </row>
@@ -16765,22 +16765,22 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>Cadiz CF</t>
+          <t>Betis</t>
         </is>
       </c>
       <c r="G178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Real Sociedad</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="I178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J178" t="n">
-        <v>4.08</v>
+        <v>2.31</v>
       </c>
       <c r="K178" t="inlineStr">
         <is>
@@ -16788,15 +16788,15 @@
         </is>
       </c>
       <c r="L178" t="n">
-        <v>6.27</v>
+        <v>2.67</v>
       </c>
       <c r="M178" t="inlineStr">
         <is>
-          <t>21/12/2023 18:57</t>
+          <t>21/12/2023 18:59</t>
         </is>
       </c>
       <c r="N178" t="n">
-        <v>3.38</v>
+        <v>3.42</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -16804,7 +16804,7 @@
         </is>
       </c>
       <c r="P178" t="n">
-        <v>3.59</v>
+        <v>3.55</v>
       </c>
       <c r="Q178" t="inlineStr">
         <is>
@@ -16812,7 +16812,7 @@
         </is>
       </c>
       <c r="R178" t="n">
-        <v>1.9</v>
+        <v>2.96</v>
       </c>
       <c r="S178" t="inlineStr">
         <is>
@@ -16820,7 +16820,7 @@
         </is>
       </c>
       <c r="T178" t="n">
-        <v>1.69</v>
+        <v>2.69</v>
       </c>
       <c r="U178" t="inlineStr">
         <is>
@@ -16829,7 +16829,7 @@
       </c>
       <c r="V178" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/cadiz-real-sociedad/6okD1TRP/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/betis-girona/Sfj929CJ/</t>
         </is>
       </c>
     </row>
@@ -16857,22 +16857,22 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>Mallorca</t>
+          <t>Alaves</t>
         </is>
       </c>
       <c r="G179" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>Osasuna</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="I179" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J179" t="n">
-        <v>2.22</v>
+        <v>4.44</v>
       </c>
       <c r="K179" t="inlineStr">
         <is>
@@ -16880,15 +16880,15 @@
         </is>
       </c>
       <c r="L179" t="n">
-        <v>2.26</v>
+        <v>6.04</v>
       </c>
       <c r="M179" t="inlineStr">
         <is>
-          <t>21/12/2023 21:29</t>
+          <t>21/12/2023 21:28</t>
         </is>
       </c>
       <c r="N179" t="n">
-        <v>3.02</v>
+        <v>3.85</v>
       </c>
       <c r="O179" t="inlineStr">
         <is>
@@ -16896,15 +16896,15 @@
         </is>
       </c>
       <c r="P179" t="n">
-        <v>2.92</v>
+        <v>4.13</v>
       </c>
       <c r="Q179" t="inlineStr">
         <is>
-          <t>21/12/2023 21:29</t>
+          <t>21/12/2023 21:27</t>
         </is>
       </c>
       <c r="R179" t="n">
-        <v>3.52</v>
+        <v>1.71</v>
       </c>
       <c r="S179" t="inlineStr">
         <is>
@@ -16912,16 +16912,16 @@
         </is>
       </c>
       <c r="T179" t="n">
-        <v>4.11</v>
+        <v>1.6</v>
       </c>
       <c r="U179" t="inlineStr">
         <is>
-          <t>21/12/2023 21:29</t>
+          <t>21/12/2023 21:19</t>
         </is>
       </c>
       <c r="V179" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/mallorca-osasuna/CSRucmzs/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/alaves-real-madrid/bqUifoKa/</t>
         </is>
       </c>
     </row>
@@ -16949,22 +16949,22 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>Alaves</t>
+          <t>Mallorca</t>
         </is>
       </c>
       <c r="G180" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Osasuna</t>
         </is>
       </c>
       <c r="I180" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J180" t="n">
-        <v>4.44</v>
+        <v>2.22</v>
       </c>
       <c r="K180" t="inlineStr">
         <is>
@@ -16972,15 +16972,15 @@
         </is>
       </c>
       <c r="L180" t="n">
-        <v>6.04</v>
+        <v>2.26</v>
       </c>
       <c r="M180" t="inlineStr">
         <is>
-          <t>21/12/2023 21:28</t>
+          <t>21/12/2023 21:29</t>
         </is>
       </c>
       <c r="N180" t="n">
-        <v>3.85</v>
+        <v>3.02</v>
       </c>
       <c r="O180" t="inlineStr">
         <is>
@@ -16988,15 +16988,15 @@
         </is>
       </c>
       <c r="P180" t="n">
-        <v>4.13</v>
+        <v>2.92</v>
       </c>
       <c r="Q180" t="inlineStr">
         <is>
-          <t>21/12/2023 21:27</t>
+          <t>21/12/2023 21:29</t>
         </is>
       </c>
       <c r="R180" t="n">
-        <v>1.71</v>
+        <v>3.52</v>
       </c>
       <c r="S180" t="inlineStr">
         <is>
@@ -17004,16 +17004,16 @@
         </is>
       </c>
       <c r="T180" t="n">
-        <v>1.6</v>
+        <v>4.11</v>
       </c>
       <c r="U180" t="inlineStr">
         <is>
-          <t>21/12/2023 21:19</t>
+          <t>21/12/2023 21:29</t>
         </is>
       </c>
       <c r="V180" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/spain/laliga/alaves-real-madrid/bqUifoKa/</t>
+          <t>https://www.betexplorer.com/football/spain/laliga/mallorca-osasuna/CSRucmzs/</t>
         </is>
       </c>
     </row>
@@ -17934,6 +17934,98 @@
       <c r="V190" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/spain/laliga/sevilla-ath-bilbao/vwSKcKQi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>spain</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>laliga</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E191" s="2" t="n">
+        <v>45295.89583333334</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Las Palmas</t>
+        </is>
+      </c>
+      <c r="G191" t="n">
+        <v>1</v>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="I191" t="n">
+        <v>2</v>
+      </c>
+      <c r="J191" t="n">
+        <v>5.24</v>
+      </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="L191" t="n">
+        <v>6.35</v>
+      </c>
+      <c r="M191" t="inlineStr">
+        <is>
+          <t>04/01/2024 21:29</t>
+        </is>
+      </c>
+      <c r="N191" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="O191" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="P191" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="Q191" t="inlineStr">
+        <is>
+          <t>04/01/2024 21:29</t>
+        </is>
+      </c>
+      <c r="R191" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="S191" t="inlineStr">
+        <is>
+          <t>17/12/2024 18:03</t>
+        </is>
+      </c>
+      <c r="T191" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="U191" t="inlineStr">
+        <is>
+          <t>04/01/2024 21:24</t>
+        </is>
+      </c>
+      <c r="V191" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/spain/laliga/las-palmas-barcelona/n3VSebe4/</t>
         </is>
       </c>
     </row>

</xml_diff>